<commit_message>
Update clipboard shortcut for item data and customer
</commit_message>
<xml_diff>
--- a/NMVS/uploads/IRQM01_Inventory request (MFG).xlsx
+++ b/NMVS/uploads/IRQM01_Inventory request (MFG).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/276815161ec3e88f/Working Space/Netmarks/Aica/Aica Docs/[u] AICA006_Inventory request upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="243" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FC1A44A-BC2B-4540-9D18-8E4F7ABCF22A}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="10_ncr:80_{98A10F0D-B2B3-47C9-A0E3-29206CDC9006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FFDFEFC-1A97-425F-9425-0FFE5D7CBD9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Item code</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>AICA AIBON 11G562-1200KG/PLASTIC TOTE(THU BỒN VỀ)</t>
-  </si>
-  <si>
-    <t>BATCH44444</t>
   </si>
 </sst>
 </file>
@@ -239,7 +236,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -254,9 +251,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -704,7 +698,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -720,16 +714,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
@@ -740,12 +734,12 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
+      <c r="B3" s="13"/>
+      <c r="C3" s="5">
+        <v>44537</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -753,31 +747,31 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="6">
+      <c r="B4" s="13"/>
+      <c r="C4" s="5">
         <f ca="1">TODAY()</f>
-        <v>44518</v>
+        <v>44537</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
@@ -786,36 +780,37 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8">
-        <v>44509</v>
+      <c r="D8" s="7">
+        <f ca="1">TODAY()</f>
+        <v>44537</v>
       </c>
       <c r="E8" s="3">
         <v>1200</v>
@@ -825,14 +820,15 @@
       <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8">
-        <v>44509</v>
+      <c r="D9" s="7">
+        <f t="shared" ref="D9:D17" ca="1" si="0">TODAY()</f>
+        <v>44537</v>
       </c>
       <c r="E9" s="3">
         <v>1200</v>
@@ -842,14 +838,15 @@
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="8">
-        <v>44509</v>
+      <c r="D10" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E10" s="3">
         <v>1200</v>
@@ -859,14 +856,15 @@
       <c r="A11" s="2">
         <v>4</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="8">
-        <v>44509</v>
+      <c r="D11" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E11" s="3">
         <v>5000</v>
@@ -876,14 +874,15 @@
       <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="8">
-        <v>44509</v>
+      <c r="D12" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E12" s="3">
         <v>13000</v>
@@ -893,14 +892,15 @@
       <c r="A13" s="2">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="8">
-        <v>44509</v>
+      <c r="D13" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E13" s="3">
         <v>1200</v>
@@ -910,14 +910,15 @@
       <c r="A14" s="2">
         <v>7</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="8">
-        <v>44509</v>
+      <c r="D14" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E14" s="3">
         <v>1200</v>
@@ -927,14 +928,15 @@
       <c r="A15" s="2">
         <v>8</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="8">
-        <v>44509</v>
+      <c r="D15" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E15" s="3">
         <v>1200</v>
@@ -944,14 +946,15 @@
       <c r="A16" s="2">
         <v>9</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="8">
-        <v>44509</v>
+      <c r="D16" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E16" s="3">
         <v>250</v>
@@ -961,26 +964,27 @@
       <c r="A17" s="2">
         <v>10</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="8">
-        <v>44509</v>
+      <c r="D17" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>44537</v>
       </c>
       <c r="E17" s="3">
         <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:F17">
@@ -993,7 +997,7 @@
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="A2:F2" xr:uid="{9FFFDF6C-E3AF-489B-8BEC-5B0E76EC9E9A}"/>
+      <autoFilter ref="A2:F2" xr:uid="{D618D6C5-7B9C-414D-AEB4-F4FA3AB04D21}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">

</xml_diff>